<commit_message>
Updated delta C master file with "three point" slope method
</commit_message>
<xml_diff>
--- a/California_Data/RES _LCMS_GC.xlsx
+++ b/California_Data/RES _LCMS_GC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8805"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Plot</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>LCMS_ppm_hr_fan_on</t>
+  </si>
+  <si>
+    <t>LCMS_ppm_hr_3point</t>
   </si>
 </sst>
 </file>
@@ -398,13 +401,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:E80">
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:F80">
+  <tableColumns count="6">
     <tableColumn id="1" name="Plot"/>
     <tableColumn id="2" name="Sensor"/>
     <tableColumn id="3" name="GC_ppm_hr"/>
     <tableColumn id="4" name="LCMS_ppm_hr"/>
     <tableColumn id="5" name="LCMS_ppm_hr_fan_on"/>
+    <tableColumn id="6" name="LCMS_ppm_hr_3point"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -614,19 +618,20 @@
   <dimension ref="A1:V80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,8 +647,11 @@
       <c r="E1" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -659,8 +667,11 @@
       <c r="E2">
         <v>64.17</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>25.625</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -676,8 +687,11 @@
       <c r="E3">
         <v>86.37</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>38.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -687,7 +701,7 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
@@ -701,7 +715,9 @@
         <v>25.65</v>
       </c>
       <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="F5" s="8">
+        <v>26.875</v>
+      </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
@@ -719,7 +735,7 @@
       <c r="U5" s="8"/>
       <c r="V5" s="8"/>
     </row>
-    <row r="6" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -732,8 +748,11 @@
       <c r="D6" s="9">
         <v>33.17</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>36.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -746,8 +765,11 @@
       <c r="D7" s="3">
         <v>29.72</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -760,8 +782,11 @@
       <c r="D8" s="4">
         <v>3.72</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>7.375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
@@ -771,7 +796,7 @@
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
     </row>
-    <row r="10" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -787,8 +812,11 @@
       <c r="E10">
         <v>29.07</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>14.0625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -804,7 +832,9 @@
       <c r="E11" s="8">
         <v>48.65</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="8">
+        <v>16.5625</v>
+      </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
@@ -822,7 +852,7 @@
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
     </row>
-    <row r="12" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -836,7 +866,9 @@
         <v>10.32</v>
       </c>
       <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+      <c r="F12" s="8">
+        <v>10.4375</v>
+      </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
@@ -854,7 +886,7 @@
       <c r="U12" s="8"/>
       <c r="V12" s="8"/>
     </row>
-    <row r="13" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -867,14 +899,17 @@
       <c r="D13" s="9">
         <v>7.79</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>9.0625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="12"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -890,8 +925,11 @@
       <c r="E15">
         <v>6.41</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -907,8 +945,11 @@
       <c r="E16">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>1.0625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>15</v>
       </c>
@@ -924,8 +965,11 @@
       <c r="E17">
         <v>5.68</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>16</v>
       </c>
@@ -941,8 +985,11 @@
       <c r="E18">
         <v>5.15</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
         <v>17</v>
       </c>
@@ -955,8 +1002,11 @@
       <c r="D19" s="1">
         <v>1.68</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>18</v>
       </c>
@@ -972,8 +1022,11 @@
       <c r="E20">
         <v>0.71</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>19</v>
       </c>
@@ -986,8 +1039,11 @@
       <c r="D21" s="1">
         <v>6.49</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="13" t="s">
         <v>20</v>
       </c>
@@ -998,8 +1054,11 @@
       <c r="D22" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>1.0625</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>21</v>
       </c>
@@ -1015,8 +1074,11 @@
       <c r="E23">
         <v>5.75</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>1.09375</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
         <v>22</v>
       </c>
@@ -1030,14 +1092,17 @@
       <c r="E24">
         <v>6.59</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
     </row>
-    <row r="26" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -1053,8 +1118,11 @@
       <c r="E26">
         <v>12.91</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>4.875</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
         <v>24</v>
       </c>
@@ -1070,8 +1138,11 @@
       <c r="E27">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>2.96875</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
         <v>25</v>
       </c>
@@ -1087,8 +1158,11 @@
       <c r="E28">
         <v>17.28</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>5.3125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
         <v>26</v>
       </c>
@@ -1104,8 +1178,11 @@
       <c r="E29">
         <v>12.11</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
         <v>27</v>
       </c>
@@ -1121,8 +1198,11 @@
       <c r="E30">
         <v>16.579999999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>4.0625</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
         <v>28</v>
       </c>
@@ -1135,8 +1215,11 @@
       <c r="D31" s="1">
         <v>7.59</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>8.4375</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
         <v>29</v>
       </c>
@@ -1152,8 +1235,11 @@
       <c r="E32">
         <v>16.07</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>4.4375</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>30</v>
       </c>
@@ -1166,8 +1252,11 @@
       <c r="D33" s="1">
         <v>15.34</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>14.625</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
         <v>31</v>
       </c>
@@ -1177,7 +1266,7 @@
       <c r="C34" s="12"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
         <v>32</v>
       </c>
@@ -1190,8 +1279,11 @@
       <c r="D35" s="1">
         <v>5.08</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>4.4375</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="13" t="s">
         <v>33</v>
       </c>
@@ -1207,8 +1299,11 @@
       <c r="E36">
         <v>9.6300000000000008</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>2.9750000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
         <v>34</v>
       </c>
@@ -1224,14 +1319,17 @@
       <c r="E37">
         <v>12.9</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>3.5625</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="12"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
     </row>
-    <row r="39" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
@@ -1245,8 +1343,11 @@
       <c r="E39">
         <v>4.6100000000000003</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
         <v>36</v>
       </c>
@@ -1260,7 +1361,7 @@
         <v>3.48</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
         <v>37</v>
       </c>
@@ -1276,8 +1377,11 @@
       <c r="E41">
         <v>13.12</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>4.375</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
         <v>38</v>
       </c>
@@ -1293,8 +1397,11 @@
       <c r="E42">
         <v>19.43</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>3.375</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
         <v>39</v>
       </c>
@@ -1310,8 +1417,11 @@
       <c r="E43">
         <v>8.1300000000000008</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="13" t="s">
         <v>40</v>
       </c>
@@ -1327,8 +1437,11 @@
       <c r="E44">
         <v>12.32</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>3.7625000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="13" t="s">
         <v>41</v>
       </c>
@@ -1341,8 +1454,11 @@
       <c r="D45" s="1">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="13" t="s">
         <v>42</v>
       </c>
@@ -1358,8 +1474,11 @@
       <c r="E46">
         <v>10.4</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>2.6875</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
         <v>43</v>
       </c>
@@ -1372,8 +1491,11 @@
       <c r="D47" s="1">
         <v>6.64</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
         <v>44</v>
       </c>
@@ -1389,8 +1511,11 @@
       <c r="E48">
         <v>12.12</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>2.1875</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>45</v>
       </c>
@@ -1400,13 +1525,13 @@
       <c r="C49" s="1"/>
       <c r="D49" s="10"/>
     </row>
-    <row r="50" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
     </row>
-    <row r="51" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>46</v>
       </c>
@@ -1422,8 +1547,11 @@
       <c r="E51">
         <v>40.11</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>9.625</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>47</v>
       </c>
@@ -1439,8 +1567,11 @@
       <c r="E52">
         <v>42.42</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>15.625</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
         <v>48</v>
       </c>
@@ -1456,8 +1587,11 @@
       <c r="E53">
         <v>19.420000000000002</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>3.5625</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
         <v>49</v>
       </c>
@@ -1473,8 +1607,11 @@
       <c r="E54">
         <v>29.83</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
         <v>50</v>
       </c>
@@ -1487,8 +1624,11 @@
       <c r="D55" s="1">
         <v>58.23</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>50.625</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
         <v>51</v>
       </c>
@@ -1504,8 +1644,11 @@
       <c r="E56">
         <v>26.23</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>6.625</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="13" t="s">
         <v>52</v>
       </c>
@@ -1515,7 +1658,7 @@
       <c r="C57" s="12"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="13" t="s">
         <v>53</v>
       </c>
@@ -1531,8 +1674,11 @@
       <c r="E58">
         <v>16.559999999999999</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>4.375</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="13" t="s">
         <v>54</v>
       </c>
@@ -1548,14 +1694,17 @@
       <c r="E59">
         <v>18.239999999999998</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>19.0625</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="12"/>
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
     </row>
-    <row r="61" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>55</v>
       </c>
@@ -1572,7 +1721,7 @@
         <v>5.75</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>56</v>
       </c>
@@ -1582,7 +1731,7 @@
       <c r="C62" s="12"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
         <v>57</v>
       </c>
@@ -1593,8 +1742,11 @@
       <c r="D63" s="1">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="13" t="s">
         <v>58</v>
       </c>
@@ -1608,7 +1760,7 @@
         <v>6.05</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
         <v>59</v>
       </c>
@@ -1621,8 +1773,11 @@
       <c r="D65" s="1">
         <v>13.89</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>22.375</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
         <v>60</v>
       </c>
@@ -1638,8 +1793,11 @@
       <c r="E66">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>2.625</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
         <v>61</v>
       </c>
@@ -1655,8 +1813,11 @@
       <c r="E67">
         <v>17.88</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="13" t="s">
         <v>62</v>
       </c>
@@ -1672,8 +1833,11 @@
       <c r="E68">
         <v>7.34</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>1.7749999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="13" t="s">
         <v>63</v>
       </c>
@@ -1689,8 +1853,11 @@
       <c r="E69">
         <v>9.24</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="13" t="s">
         <v>64</v>
       </c>
@@ -1706,14 +1873,17 @@
       <c r="E70">
         <v>10.81</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="12"/>
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
       <c r="D71" s="12"/>
     </row>
-    <row r="72" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>65</v>
       </c>
@@ -1729,8 +1899,11 @@
       <c r="E72">
         <v>45.36</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>66</v>
       </c>
@@ -1746,8 +1919,11 @@
       <c r="E73">
         <v>40</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <v>8.875</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="13" t="s">
         <v>67</v>
       </c>
@@ -1763,8 +1939,11 @@
       <c r="E74">
         <v>27.41</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="13" t="s">
         <v>68</v>
       </c>
@@ -1777,8 +1956,11 @@
       <c r="D75" s="1">
         <v>18.93</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <v>16.4375</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
         <v>69</v>
       </c>
@@ -1794,8 +1976,11 @@
       <c r="E76">
         <v>13.34</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
         <v>70</v>
       </c>
@@ -1811,8 +1996,11 @@
       <c r="E77">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="13" t="s">
         <v>71</v>
       </c>
@@ -1826,7 +2014,7 @@
         <v>2.65</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
         <v>72</v>
       </c>
@@ -1842,8 +2030,11 @@
       <c r="E79">
         <v>8.89</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <v>2.4375</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
         <v>73</v>
       </c>
@@ -1858,6 +2049,9 @@
       </c>
       <c r="E80">
         <v>2.0499999999999998</v>
+      </c>
+      <c r="F80">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>